<commit_message>
CRUD terminé tickets + utilisateurs + fix heures
</commit_message>
<xml_diff>
--- a/heures.xlsx
+++ b/heures.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -474,9 +474,17 @@
         <v>2.5</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>29/01/2024</v>
+      </c>
+      <c r="B10" t="str">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B9"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B10"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
CRUD perm, statuts, roles back & front + icons front + améliorations + patch token
</commit_message>
<xml_diff>
--- a/heures.xlsx
+++ b/heures.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -479,12 +479,28 @@
         <v>29/01/2024</v>
       </c>
       <c r="B10" t="str">
-        <v>2</v>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>30/01/2024</v>
+      </c>
+      <c r="B11" t="str">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>31/01/2024</v>
+      </c>
+      <c r="B12" t="str">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B10"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B12"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
bdd online + status + permissions + scss
</commit_message>
<xml_diff>
--- a/heures.xlsx
+++ b/heures.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -409,6 +409,9 @@
       <c r="B1" t="str">
         <v>Heures passées</v>
       </c>
+      <c r="D1" t="str">
+        <v>Total Heures</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -417,6 +420,9 @@
       <c r="B2" t="str">
         <v>2</v>
       </c>
+      <c r="D2" t="str">
+        <v>=SUM(B2:B13)</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -498,9 +504,22 @@
         <v>5</v>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>01/02/2024</v>
+      </c>
+      <c r="B13" t="str">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B12"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D14"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Refactorisation du scss + docs 1.0 + hebergement projet + connection pool
</commit_message>
<xml_diff>
--- a/heures.xlsx
+++ b/heures.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -421,7 +421,7 @@
         <v>2</v>
       </c>
       <c r="D2" t="str">
-        <v>=SUM(B2:B13)</v>
+        <v>=SUM(B2:B17)</v>
       </c>
     </row>
     <row r="3">
@@ -513,13 +513,40 @@
       </c>
     </row>
     <row r="14">
+      <c r="A14" t="str">
+        <v>05/02/2024</v>
+      </c>
       <c r="B14" t="str">
-        <v/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>06/02/2024</v>
+      </c>
+      <c r="B15" t="str">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>07/02/2024</v>
+      </c>
+      <c r="B16" t="str">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>08/02/2024</v>
+      </c>
+      <c r="B17" t="str">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D14"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D17"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update total des heures
</commit_message>
<xml_diff>
--- a/heures.xlsx
+++ b/heures.xlsx
@@ -1,41 +1,72 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mineon\Desktop\public_sae\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01549F80-CA80-40BC-A15F-ECEF19A68DEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Heures passées</t>
+  </si>
+  <si>
+    <t>###  2eme revue  ###</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Création d'un planner pour suivre les tâches du projet</t>
+  </si>
+  <si>
+    <t>Total Heures (2eme revue)</t>
+  </si>
+  <si>
+    <t>Total Heures (1ere revue)</t>
+  </si>
+  <si>
+    <t>Total Heures Global</t>
+  </si>
+  <si>
+    <t>Ajout de tâches dans le planner &amp; modification fichier excel</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -64,14 +95,38 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -396,197 +451,262 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.75" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Date</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Heures passées</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Total Heures</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>17/12/2023</v>
-      </c>
-      <c r="B2" t="str">
+    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>45277</v>
+      </c>
+      <c r="B2" s="1">
         <v>2</v>
       </c>
-      <c r="D2" t="str">
-        <v>=SUM(B2:B22)</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>15/01/2024</v>
-      </c>
-      <c r="B3" t="str">
+      <c r="E2" s="1">
+        <f>SUM(B2:B22)</f>
+        <v>120</v>
+      </c>
+      <c r="G2">
+        <f>SUM(B25:B26)</f>
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <f>SUM(E2,G2)</f>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>45306</v>
+      </c>
+      <c r="B3" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>19/01/2024</v>
-      </c>
-      <c r="B4" t="str">
+    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>45310</v>
+      </c>
+      <c r="B4" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>22/01/2024</v>
-      </c>
-      <c r="B5" t="str">
+    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>45313</v>
+      </c>
+      <c r="B5" s="1">
         <v>0.5</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>23/01/2024</v>
-      </c>
-      <c r="B6" t="str">
+    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>45314</v>
+      </c>
+      <c r="B6" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>25/01/2024</v>
-      </c>
-      <c r="B7" t="str">
+    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>45316</v>
+      </c>
+      <c r="B7" s="1">
         <v>1.5</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>27/01/2024</v>
-      </c>
-      <c r="B8" t="str">
+    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>45318</v>
+      </c>
+      <c r="B8" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>28/01/2024</v>
-      </c>
-      <c r="B9" t="str">
+    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>45319</v>
+      </c>
+      <c r="B9" s="1">
         <v>2.5</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>29/01/2024</v>
-      </c>
-      <c r="B10" t="str">
+    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>45320</v>
+      </c>
+      <c r="B10" s="1">
         <v>4.5</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="str">
-        <v>30/01/2024</v>
-      </c>
-      <c r="B11" t="str">
+    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>45321</v>
+      </c>
+      <c r="B11" s="1">
         <v>3.5</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="str">
-        <v>31/01/2024</v>
-      </c>
-      <c r="B12" t="str">
+    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>45322</v>
+      </c>
+      <c r="B12" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="str">
-        <v>01/02/2024</v>
-      </c>
-      <c r="B13" t="str">
+    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>45323</v>
+      </c>
+      <c r="B13" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="str">
-        <v>05/02/2024</v>
-      </c>
-      <c r="B14" t="str">
+    <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>45327</v>
+      </c>
+      <c r="B14" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="str">
-        <v>06/02/2024</v>
-      </c>
-      <c r="B15" t="str">
+    <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>45328</v>
+      </c>
+      <c r="B15" s="1">
         <v>9</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="str">
-        <v>07/02/2024</v>
-      </c>
-      <c r="B16" t="str">
+    <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>45329</v>
+      </c>
+      <c r="B16" s="1">
         <v>11</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="str">
-        <v>08/02/2024</v>
-      </c>
-      <c r="B17" t="str">
+    <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>45330</v>
+      </c>
+      <c r="B17" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" t="str">
-        <v>09/02/2024</v>
-      </c>
-      <c r="B18" t="str">
+    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>45331</v>
+      </c>
+      <c r="B18" s="1">
         <v>9</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" t="str">
-        <v>10/02/2024</v>
-      </c>
-      <c r="B19" t="str">
+    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>45332</v>
+      </c>
+      <c r="B19" s="1">
         <v>11</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" t="str">
-        <v>11/02/2024</v>
-      </c>
-      <c r="B20" t="str">
+    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>45333</v>
+      </c>
+      <c r="B20" s="1">
         <v>11</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" t="str">
-        <v>12/02/2024</v>
-      </c>
-      <c r="B21" t="str">
+    <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>45334</v>
+      </c>
+      <c r="B21" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" t="str">
-        <v>13/02/2024</v>
-      </c>
-      <c r="B22" t="str">
+    <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>45335</v>
+      </c>
+      <c r="B22" s="1">
         <v>7.5</v>
       </c>
     </row>
+    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="6"/>
+      <c r="C24" s="8"/>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <v>45368</v>
+      </c>
+      <c r="B25" s="7">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
+        <v>45369</v>
+      </c>
+      <c r="B26" s="7">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A24:B24"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D22"/>
+    <ignoredError sqref="A1:B1 D3 D4 D5 D6 D7 D8 D9 D10 D11 D12 D13 D14 D15 D16 D17 D18 D19 D20 D21 D22" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update heures + détail des heures
</commit_message>
<xml_diff>
--- a/heures.xlsx
+++ b/heures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mineon\Desktop\public_sae\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01549F80-CA80-40BC-A15F-ECEF19A68DEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94D52513-03DC-4C30-ABFD-DE45692785C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -60,6 +60,12 @@
   </si>
   <si>
     <t>Ajout de tâches dans le planner &amp; modification fichier excel</t>
+  </si>
+  <si>
+    <t>Ajout en base de données d'une colonne qui spécifie le rôle par défaut ou non. Modification de l'API pour empêcher la modification d'un rôle par défaut. Ajout d'un cadenas rouge bloqué et vert débloqué pour différencier les deux</t>
+  </si>
+  <si>
+    <t>Maintenance du planner</t>
   </si>
 </sst>
 </file>
@@ -95,9 +101,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -105,14 +110,9 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,34 +452,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.375" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="190.75" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.75" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G1" t="s">
@@ -489,214 +489,236 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>45277</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2">
         <v>2</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2">
         <f>SUM(B2:B22)</f>
         <v>120</v>
       </c>
       <c r="G2">
-        <f>SUM(B25:B26)</f>
-        <v>2</v>
+        <f>SUM(B25:B27)</f>
+        <v>3</v>
       </c>
       <c r="I2">
         <f>SUM(E2,G2)</f>
-        <v>122</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
         <v>45306</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
         <v>45310</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
         <v>45313</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5">
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
         <v>45314</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
         <v>45316</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7">
         <v>1.5</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
         <v>45318</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
         <v>45319</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9">
         <v>2.5</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
         <v>45320</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10">
         <v>4.5</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
         <v>45321</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11">
         <v>3.5</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
         <v>45322</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
         <v>45323</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
         <v>45327</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
         <v>45328</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
         <v>45329</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
         <v>45330</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
         <v>45331</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
         <v>45332</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
         <v>45333</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
         <v>45334</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
         <v>45335</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22">
         <v>7.5</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="8"/>
-    </row>
-    <row r="25" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
+      <c r="B24" s="4"/>
+      <c r="C24" s="2"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
         <v>45368</v>
       </c>
-      <c r="B25" s="7">
+      <c r="B25">
         <v>1</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
         <v>45369</v>
       </c>
-      <c r="B26" s="7">
+      <c r="B26">
         <v>1</v>
       </c>
       <c r="C26" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>45369</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>45369</v>
+      </c>
+      <c r="B28">
+        <v>0.5</v>
+      </c>
+      <c r="C28" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>